<commit_message>
added excel file for testing
</commit_message>
<xml_diff>
--- a/assignment5/part1/Assignment5_testing_times.xlsx
+++ b/assignment5/part1/Assignment5_testing_times.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/divitkoradia/Google Drive/CS4500/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83EC11FF-EDE1-D649-A2B4-F5E9118D1F1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EBC0F7-4D43-664D-A694-6E33A94D88B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{939B2658-ABA8-2A48-890C-5B4DD44F7449}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rower 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>map</t>
   </si>
@@ -41,15 +41,6 @@
     <t>pmap</t>
   </si>
   <si>
-    <t>Test 1</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>Test 3</t>
-  </si>
-  <si>
     <t>File info</t>
   </si>
   <si>
@@ -65,17 +56,48 @@
     <t>120 MB</t>
   </si>
   <si>
-    <t xml:space="preserve">Len </t>
+    <t>max_length = approx 3.5 millions rows</t>
+  </si>
+  <si>
+    <t>Ethan MacBook Pro Specs</t>
+  </si>
+  <si>
+    <t>Test 1(s)</t>
+  </si>
+  <si>
+    <t>Test 2(s)</t>
+  </si>
+  <si>
+    <t>Test 3(s)</t>
+  </si>
+  <si>
+    <t>2.2 GHz Quad-Core Intel Core i7</t>
+  </si>
+  <si>
+    <t>16GB RAM</t>
+  </si>
+  <si>
+    <t>half_length = approx 1.75 millions rows</t>
+  </si>
+  <si>
+    <t>1/10_length = approx 350,000  rows</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,8 +123,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,60 +443,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D46A82-6803-6A4C-BB62-5785EF954C79}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>97.04</v>
+      </c>
+      <c r="C3" s="1">
+        <v>96.48</v>
+      </c>
+      <c r="D3" s="1">
+        <v>97.09</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>59.244</v>
+      </c>
+      <c r="C4" s="1">
+        <v>60.68</v>
+      </c>
+      <c r="D4" s="1">
+        <v>58.996000000000002</v>
+      </c>
+      <c r="I4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B8" s="1">
+        <v>48.542999999999999</v>
+      </c>
+      <c r="C8" s="1">
+        <v>48.154000000000003</v>
+      </c>
+      <c r="D8" s="1">
+        <v>48.031999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G6" t="s">
+      <c r="B9" s="1">
+        <v>27.18</v>
+      </c>
+      <c r="C9" s="1">
+        <v>27.835000000000001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>27.783000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>8.9260000000000002</v>
+      </c>
+      <c r="C13" s="1">
+        <v>9.23</v>
+      </c>
+      <c r="D13" s="1">
+        <v>9.1539999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5.7080000000000002</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5.5730000000000004</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5.5780000000000003</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A11:D11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made changes to memo and excel file
</commit_message>
<xml_diff>
--- a/assignment5/part1/Assignment5_testing_times.xlsx
+++ b/assignment5/part1/Assignment5_testing_times.xlsx
@@ -5,17 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/divitkoradia/Google Drive/CS4500/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/divitkoradia/Google Drive/CS4500/Homework/SoftwareDev (1)/assignment5/part1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EBC0F7-4D43-664D-A694-6E33A94D88B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1FD6AD-B1E1-374F-904B-F5DD3957ADD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{939B2658-ABA8-2A48-890C-5B4DD44F7449}"/>
   </bookViews>
   <sheets>
     <sheet name="Rower 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">'Rower 1'!$K$2</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Rower 1'!$K$3</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Rower 1'!$L$1:$N$1</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Rower 1'!$L$2:$N$2</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'Rower 1'!$L$3:$N$3</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>map</t>
   </si>
@@ -82,12 +89,27 @@
   <si>
     <t>1/10_length = approx 350,000  rows</t>
   </si>
+  <si>
+    <t>half_len</t>
+  </si>
+  <si>
+    <t>max_len</t>
+  </si>
+  <si>
+    <t>one_tenth_len</t>
+  </si>
+  <si>
+    <t>Avg(s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,6 +120,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,12 +152,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,6 +178,1177 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> t</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> taken to run Rower 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Rower 1'!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Rower 1'!$L$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>max_len</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>half_len</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>one_tenth_len</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Rower 1'!$L$2:$N$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>96.87</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48.243000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1033000000000008</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-79E9-3F47-815D-59FEDA76E68E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Rower 1'!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pmap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Rower 1'!$L$1:$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>max_len</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>half_len</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>one_tenth_len</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Rower 1'!$L$3:$N$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>59.64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.593330000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6196599999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-79E9-3F47-815D-59FEDA76E68E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1386377232"/>
+        <c:axId val="1386587264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1386377232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1386587264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1386587264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1386377232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CF5B7D0-1AF1-0B4A-8E4A-96EE148A84C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,10 +1648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D46A82-6803-6A4C-BB62-5785EF954C79}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B28" sqref="B28:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,23 +1659,34 @@
     <col min="6" max="6" width="27.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -481,14 +1697,29 @@
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>96.87</v>
+      </c>
+      <c r="M2" s="3">
+        <v>48.243000000000002</v>
+      </c>
+      <c r="N2" s="3">
+        <v>9.1033000000000008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,14 +1732,30 @@
       <c r="D3" s="1">
         <v>97.09</v>
       </c>
+      <c r="E3" s="1">
+        <f>AVERAGE(B3:D3)</f>
+        <v>96.87</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <v>59.64</v>
+      </c>
+      <c r="M3" s="3">
+        <v>27.593330000000002</v>
+      </c>
+      <c r="N3" s="3">
+        <v>5.6196599999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -521,24 +1768,34 @@
       <c r="D4" s="1">
         <v>58.996000000000002</v>
       </c>
-      <c r="I4" t="s">
+      <c r="E4" s="1">
+        <f>AVERAGE(B4:D4)</f>
+        <v>59.640000000000008</v>
+      </c>
+      <c r="G4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I5" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="G5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -549,8 +1806,11 @@
       <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,8 +1823,12 @@
       <c r="D8" s="1">
         <v>48.031999999999996</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E8" s="1">
+        <f>AVERAGE(B8:D8)</f>
+        <v>48.242999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -577,16 +1841,28 @@
       <c r="D9" s="1">
         <v>27.783000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E9" s="1">
+        <f>AVERAGE(B9:D9)</f>
+        <v>27.599333333333334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>9</v>
@@ -597,8 +1873,11 @@
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,8 +1890,12 @@
       <c r="D13" s="1">
         <v>9.1539999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E13" s="1">
+        <f>AVERAGE(B13:D13)</f>
+        <v>9.1033333333333335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -625,13 +1908,179 @@
       <c r="D14" s="1">
         <v>5.5780000000000003</v>
       </c>
+      <c r="E14" s="1">
+        <f>AVERAGE(B14:D14)</f>
+        <v>5.6196666666666673</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="e">
+        <f>AVERAGE(B18:D18)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="e">
+        <f>AVERAGE(B19:D19)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5" t="e">
+        <f>AVERAGE(B23:D23)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="e">
+        <f>AVERAGE(B24:D24)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="e">
+        <f>AVERAGE(B28:D28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="e">
+        <f>AVERAGE(B29:D29)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A26:D26"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated excel sheet. Rower 1 complete
</commit_message>
<xml_diff>
--- a/assignment5/part1/Assignment5_testing_times.xlsx
+++ b/assignment5/part1/Assignment5_testing_times.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/divitkoradia/Google Drive/CS4500/Homework/SoftwareDev (1)/assignment5/part1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA93B9E8-F6F0-5D49-B667-0A2C56842E3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80448D3-19EA-6944-A1F8-68E234D910DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{939B2658-ABA8-2A48-890C-5B4DD44F7449}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{939B2658-ABA8-2A48-890C-5B4DD44F7449}"/>
   </bookViews>
   <sheets>
     <sheet name="Rower 1" sheetId="1" r:id="rId1"/>
     <sheet name="Rower 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">'Rower 1'!$K$2</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'Rower 1'!$K$3</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'Rower 1'!$L$1:$N$1</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'Rower 1'!$L$2:$N$2</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">'Rower 1'!$L$3:$N$3</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'Rower 1'!$K$7</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Rower 1'!$K$8</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Rower 1'!$L$6:$N$6</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Rower 1'!$L$7:$N$7</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'Rower 1'!$L$8:$N$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="20">
   <si>
     <t>map</t>
   </si>
@@ -153,17 +153,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -768,7 +769,641 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Average time taken to run Rower 1 Divit</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11612456747404844"/>
+          <c:y val="0.12145038500021751"/>
+          <c:w val="0.8648442906574394"/>
+          <c:h val="0.7513113933962674"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Rower 1'!$K$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>map</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Rower 1'!$L$6:$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>max_len</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>half_len</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>one_tenth_len</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Rower 1'!$L$7:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>60.44</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.446000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2933000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8871-D440-832A-A8F686F439E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Rower 1'!$K$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pmap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Rower 1'!$L$6:$N$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>max_len</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>half_len</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>one_tenth_len</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Rower 1'!$L$8:$N$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>39.122999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.046600000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0853333300000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8871-D440-832A-A8F686F439E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1423825760"/>
+        <c:axId val="1387502400"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1423825760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1387502400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1387502400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.5570934256055362E-2"/>
+              <c:y val="0.44531735328664029"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1423825760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1311,20 +1946,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>488950</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1344,6 +2482,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1016000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48625D81-5C2F-1D43-909D-702BFAF37906}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1651,8 +2825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D46A82-6803-6A4C-BB62-5785EF954C79}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1677,13 +2851,14 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1707,16 +2882,16 @@
       <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="6">
         <v>96.87</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="6">
         <v>48.243000000000002</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="6">
         <v>9.1033000000000008</v>
       </c>
     </row>
@@ -1743,16 +2918,16 @@
       <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="6">
         <v>59.64</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="6">
         <v>27.593330000000002</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="6">
         <v>5.6196599999999997</v>
       </c>
     </row>
@@ -1795,6 +2970,16 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
@@ -1810,6 +2995,18 @@
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="K7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>60.44</v>
+      </c>
+      <c r="M7" s="5">
+        <v>31.446000000000002</v>
+      </c>
+      <c r="N7" s="5">
+        <v>6.2933000000000003</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -1827,6 +3024,18 @@
       <c r="E8" s="1">
         <f>AVERAGE(B8:D8)</f>
         <v>48.242999999999995</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="5">
+        <v>39.122999999999998</v>
+      </c>
+      <c r="M8" s="5">
+        <v>20.046600000000002</v>
+      </c>
+      <c r="N8" s="5">
+        <v>4.0853333300000001</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1915,175 +3124,197 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="e">
+      <c r="B18" s="4">
+        <v>60.42</v>
+      </c>
+      <c r="C18" s="4">
+        <v>60.51</v>
+      </c>
+      <c r="D18" s="4">
+        <v>60.39</v>
+      </c>
+      <c r="E18" s="4">
         <f>AVERAGE(B18:D18)</f>
-        <v>#DIV/0!</v>
+        <v>60.44</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="e">
+      <c r="B19" s="4">
+        <v>40.07</v>
+      </c>
+      <c r="C19" s="4">
+        <v>38.493000000000002</v>
+      </c>
+      <c r="D19" s="4">
+        <v>38.807000000000002</v>
+      </c>
+      <c r="E19" s="4">
         <f>AVERAGE(B19:D19)</f>
-        <v>#DIV/0!</v>
+        <v>39.123333333333335</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="5">
-        <v>160.88</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5">
+      <c r="B23" s="4">
+        <v>31.454000000000001</v>
+      </c>
+      <c r="C23" s="4">
+        <v>30.596</v>
+      </c>
+      <c r="D23" s="4">
+        <v>32.287999999999997</v>
+      </c>
+      <c r="E23" s="4">
         <f>AVERAGE(B23:D23)</f>
-        <v>160.88</v>
+        <v>31.445999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5" t="e">
+      <c r="B24" s="4">
+        <v>20.870999999999999</v>
+      </c>
+      <c r="C24" s="4">
+        <v>19.565999999999999</v>
+      </c>
+      <c r="D24" s="4">
+        <v>19.702999999999999</v>
+      </c>
+      <c r="E24" s="4">
         <f>AVERAGE(B24:D24)</f>
-        <v>#DIV/0!</v>
+        <v>20.046666666666667</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="5">
-        <v>13.282999999999999</v>
-      </c>
-      <c r="C28" s="5">
-        <v>13.103999999999999</v>
-      </c>
-      <c r="D28" s="5">
-        <v>13.041</v>
-      </c>
-      <c r="E28" s="5">
+      <c r="B28" s="4">
+        <v>6.6070000000000002</v>
+      </c>
+      <c r="C28" s="4">
+        <v>6.1269999999999998</v>
+      </c>
+      <c r="D28" s="4">
+        <v>6.1459999999999999</v>
+      </c>
+      <c r="E28" s="4">
         <f>AVERAGE(B28:D28)</f>
-        <v>13.142666666666665</v>
+        <v>6.293333333333333</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="5">
-        <v>12.827999999999999</v>
-      </c>
-      <c r="C29" s="5">
-        <v>12.635</v>
-      </c>
-      <c r="D29" s="5">
-        <v>12.601000000000001</v>
-      </c>
-      <c r="E29" s="5">
+      <c r="B29" s="4">
+        <v>4.0629999999999997</v>
+      </c>
+      <c r="C29" s="4">
+        <v>4.0250000000000004</v>
+      </c>
+      <c r="D29" s="4">
+        <v>4.1680000000000001</v>
+      </c>
+      <c r="E29" s="4">
         <f>AVERAGE(B29:D29)</f>
-        <v>12.688000000000001</v>
+        <v>4.0853333333333337</v>
       </c>
     </row>
   </sheetData>
@@ -2104,7 +3335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1C4041-F5C5-8343-8BB9-CBD6597837B7}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -2269,159 +3500,159 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5" t="e">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="e">
         <f>AVERAGE(B18:D18)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="e">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="e">
         <f>AVERAGE(B19:D19)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5" t="s">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5" t="e">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="e">
         <f>AVERAGE(B23:D23)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5" t="e">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4" t="e">
         <f>AVERAGE(B24:D24)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5" t="s">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5" t="e">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4" t="e">
         <f>AVERAGE(B28:D28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="e">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="e">
         <f>AVERAGE(B29:D29)</f>
         <v>#DIV/0!</v>
       </c>

</xml_diff>

<commit_message>
updated time excel sheet
</commit_message>
<xml_diff>
--- a/assignment5/part1/Assignment5_testing_times.xlsx
+++ b/assignment5/part1/Assignment5_testing_times.xlsx
@@ -8,21 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/divitkoradia/Google Drive/CS4500/Homework/SoftwareDev (1)/assignment5/part1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80448D3-19EA-6944-A1F8-68E234D910DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6788EF5-A44E-A847-BD87-4B7CF1AC1CFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{939B2658-ABA8-2A48-890C-5B4DD44F7449}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{939B2658-ABA8-2A48-890C-5B4DD44F7449}"/>
   </bookViews>
   <sheets>
     <sheet name="Rower 1" sheetId="1" r:id="rId1"/>
     <sheet name="Rower 2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">'Rower 1'!$K$7</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'Rower 1'!$K$8</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'Rower 1'!$L$6:$N$6</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'Rower 1'!$L$7:$N$7</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">'Rower 1'!$L$8:$N$8</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -156,15 +149,15 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2825,7 +2818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D46A82-6803-6A4C-BB62-5785EF954C79}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -2838,12 +2831,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -2885,13 +2878,13 @@
       <c r="K2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="4">
         <v>96.87</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="4">
         <v>48.243000000000002</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="4">
         <v>9.1033000000000008</v>
       </c>
     </row>
@@ -2921,13 +2914,13 @@
       <c r="K3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="4">
         <v>59.64</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="4">
         <v>27.593330000000002</v>
       </c>
-      <c r="N3" s="6">
+      <c r="N3" s="4">
         <v>5.6196599999999997</v>
       </c>
     </row>
@@ -2963,21 +2956,21 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="1"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4" t="s">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2995,16 +2988,16 @@
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="3">
         <v>60.44</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="3">
         <v>31.446000000000002</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="3">
         <v>6.2933000000000003</v>
       </c>
     </row>
@@ -3025,16 +3018,16 @@
         <f>AVERAGE(B8:D8)</f>
         <v>48.242999999999995</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="3">
         <v>39.122999999999998</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="3">
         <v>20.046600000000002</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="3">
         <v>4.0853333300000001</v>
       </c>
     </row>
@@ -3064,12 +3057,12 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -3124,195 +3117,195 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="2">
         <v>60.42</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="2">
         <v>60.51</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="2">
         <v>60.39</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="2">
         <f>AVERAGE(B18:D18)</f>
         <v>60.44</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="2">
         <v>40.07</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="2">
         <v>38.493000000000002</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="2">
         <v>38.807000000000002</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="2">
         <f>AVERAGE(B19:D19)</f>
         <v>39.123333333333335</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B23" s="2">
         <v>31.454000000000001</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="2">
         <v>30.596</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="2">
         <v>32.287999999999997</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="2">
         <f>AVERAGE(B23:D23)</f>
         <v>31.445999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="4">
+      <c r="B24" s="2">
         <v>20.870999999999999</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="2">
         <v>19.565999999999999</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="2">
         <v>19.702999999999999</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="2">
         <f>AVERAGE(B24:D24)</f>
         <v>20.046666666666667</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="2">
         <v>6.6070000000000002</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="2">
         <v>6.1269999999999998</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="2">
         <v>6.1459999999999999</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="2">
         <f>AVERAGE(B28:D28)</f>
         <v>6.293333333333333</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="2">
         <v>4.0629999999999997</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="2">
         <v>4.0250000000000004</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="2">
         <v>4.1680000000000001</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="2">
         <f>AVERAGE(B29:D29)</f>
         <v>4.0853333333333337</v>
       </c>
@@ -3335,19 +3328,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1C4041-F5C5-8343-8BB9-CBD6597837B7}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3397,12 +3390,12 @@
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3452,12 +3445,12 @@
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3500,171 +3493,191 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="e">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="e">
         <f>AVERAGE(B18:D18)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4" t="e">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="e">
         <f>AVERAGE(B19:D19)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4" t="e">
+      <c r="B23" s="2">
+        <v>11.704000000000001</v>
+      </c>
+      <c r="C23" s="2">
+        <v>11.667</v>
+      </c>
+      <c r="D23" s="2">
+        <v>11.45</v>
+      </c>
+      <c r="E23" s="2">
         <f>AVERAGE(B23:D23)</f>
-        <v>#DIV/0!</v>
+        <v>11.606999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4" t="e">
+      <c r="B24" s="2">
+        <v>9.9760000000000009</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2">
         <f>AVERAGE(B24:D24)</f>
-        <v>#DIV/0!</v>
+        <v>9.9760000000000009</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4" t="s">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4" t="e">
+      <c r="B28" s="2">
+        <v>2.3879999999999999</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2.331</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2.3439999999999999</v>
+      </c>
+      <c r="E28" s="2">
         <f>AVERAGE(B28:D28)</f>
-        <v>#DIV/0!</v>
+        <v>2.3543333333333329</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4" t="e">
+      <c r="B29" s="2">
+        <v>2.17</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2.097</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2.0960000000000001</v>
+      </c>
+      <c r="E29" s="2">
         <f>AVERAGE(B29:D29)</f>
-        <v>#DIV/0!</v>
+        <v>2.121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A26:D26"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>